<commit_message>
Registrar Oferta del fabricante
</commit_message>
<xml_diff>
--- a/CSOF5303 Proyecto 3/Ciclo2/5DS_AplicacionesLegado.xlsx
+++ b/CSOF5303 Proyecto 3/Ciclo2/5DS_AplicacionesLegado.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="80">
   <si>
     <t>PoManager</t>
   </si>
@@ -250,6 +250,15 @@
   </si>
   <si>
     <t>El metodo que retorna las subastas de un fabricante no verifica que todavia este abierta</t>
+  </si>
+  <si>
+    <t>El unico criterio actual es el mejor precio, el metodo de dar ganador no tiene sentido, el mejor se asigna cada vez que se registra una nueva oferta</t>
+  </si>
+  <si>
+    <t>Al registrar la oferta no se estaba asignando a la subasta correspondiente</t>
+  </si>
+  <si>
+    <t>El metodo de registrar oferta estaba en el bean pero no en el web service y por tanto nunca era empleado</t>
   </si>
 </sst>
 </file>
@@ -1464,10 +1473,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:C12"/>
+  <dimension ref="B2:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1514,19 +1523,34 @@
         <v>76</v>
       </c>
     </row>
+    <row r="9" spans="2:3">
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
+    </row>
     <row r="10" spans="2:3">
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="C11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" t="s">
         <v>69</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="2:3">
-      <c r="B12" t="s">
+    <row r="15" spans="2:3">
+      <c r="B15" t="s">
         <v>71</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C15" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
consultar fabricantes de subasta y cerrar subasta
</commit_message>
<xml_diff>
--- a/CSOF5303 Proyecto 3/Ciclo2/5DS_AplicacionesLegado.xlsx
+++ b/CSOF5303 Proyecto 3/Ciclo2/5DS_AplicacionesLegado.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="11715" windowHeight="7200" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="11715" windowHeight="7200"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="82">
   <si>
     <t>PoManager</t>
   </si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>El metodo de registrar oferta estaba en el bean pero no en el web service y por tanto nunca era empleado</t>
+  </si>
+  <si>
+    <t>Muchos de los metodos no usan la implementacion del toBO por tanto se pueden generar muchos errores al momento de mapear la info</t>
+  </si>
+  <si>
+    <t>El metodo de cerrar subasta no esta persistiendo los cambios</t>
   </si>
 </sst>
 </file>
@@ -706,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1473,10 +1479,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:C15"/>
+  <dimension ref="B2:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1538,24 +1544,35 @@
         <v>79</v>
       </c>
     </row>
+    <row r="12" spans="2:3">
+      <c r="C12" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="13" spans="2:3">
-      <c r="B13" t="s">
-        <v>69</v>
-      </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="2:3">
       <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
         <v>71</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Agregada la consulta a los web services de fedex
</commit_message>
<xml_diff>
--- a/CSOF5303 Proyecto 3/Ciclo2/5DS_AplicacionesLegado.xlsx
+++ b/CSOF5303 Proyecto 3/Ciclo2/5DS_AplicacionesLegado.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="11715" windowHeight="7200"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="11715" windowHeight="7200" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="84">
   <si>
     <t>PoManager</t>
   </si>
@@ -265,6 +265,12 @@
   </si>
   <si>
     <t>El metodo de cerrar subasta no esta persistiendo los cambios</t>
+  </si>
+  <si>
+    <t>Los campos de fecha en la base de datos estan como Date, lo cual impide que se almacene la hora, se cambian a datetime</t>
+  </si>
+  <si>
+    <t>El mapeo de hibernate tiene los campos fecha como DATE se cambian a TIMESTAMP</t>
   </si>
 </sst>
 </file>
@@ -712,7 +718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
@@ -1479,10 +1485,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:C17"/>
+  <dimension ref="B2:C19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1554,19 +1560,29 @@
         <v>81</v>
       </c>
     </row>
+    <row r="14" spans="2:3">
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
+    </row>
     <row r="15" spans="2:3">
-      <c r="B15" t="s">
-        <v>69</v>
-      </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
         <v>71</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Documentacion base de datos legado
</commit_message>
<xml_diff>
--- a/CSOF5303 Proyecto 3/Ciclo2/5DS_AplicacionesLegado.xlsx
+++ b/CSOF5303 Proyecto 3/Ciclo2/5DS_AplicacionesLegado.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="11715" windowHeight="7200" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="11715" windowHeight="7200"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Datos!$B$2:$F$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Datos!$B$2:$F$74</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="104">
   <si>
     <t>PoManager</t>
   </si>
@@ -271,6 +271,66 @@
   </si>
   <si>
     <t>El mapeo de hibernate tiene los campos fecha como DATE se cambian a TIMESTAMP</t>
+  </si>
+  <si>
+    <t>codPostal</t>
+  </si>
+  <si>
+    <t>codPais</t>
+  </si>
+  <si>
+    <t>Necesario para el envio</t>
+  </si>
+  <si>
+    <t>Nuevo : Necesario para el overhead</t>
+  </si>
+  <si>
+    <t>Nuevo : Para informar sobre el estado de la subasta</t>
+  </si>
+  <si>
+    <t>Necesario para informar sobre el estado de la oferta</t>
+  </si>
+  <si>
+    <t>mensaje</t>
+  </si>
+  <si>
+    <t>estadoOferta</t>
+  </si>
+  <si>
+    <t>Nuevo : Contiene la informacion de costo de envio</t>
+  </si>
+  <si>
+    <t>Nuevo : Indica si la oferta es la mejor o fue superada</t>
+  </si>
+  <si>
+    <t>Nuevo : Para calcular el overhead</t>
+  </si>
+  <si>
+    <t>peso</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>Modificado : Para almacenar la hora</t>
+  </si>
+  <si>
+    <t>fechaCreacionSubasta</t>
+  </si>
+  <si>
+    <t>fechaMaxSubasta</t>
+  </si>
+  <si>
+    <t>Nuevo : Resumen de la oferta ganadora</t>
+  </si>
+  <si>
+    <t>Nuevo : Fecha en la que se crea la subasta</t>
+  </si>
+  <si>
+    <t>Nuevo : Fecha maxima para ofertar</t>
+  </si>
+  <si>
+    <t>Modificado : Se cambia la llave unica</t>
   </si>
 </sst>
 </file>
@@ -294,7 +354,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,8 +373,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -374,11 +446,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -420,6 +523,30 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -716,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:F62"/>
+  <dimension ref="B2:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -729,7 +856,7 @@
     <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49.85546875" style="1" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -774,7 +901,9 @@
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="10"/>
@@ -803,99 +932,105 @@
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="11"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="4" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="4"/>
+      <c r="E7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="10"/>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="3"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="10"/>
-      <c r="C10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="3"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="10"/>
+      <c r="B11" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="C11" s="3" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="10"/>
       <c r="C12" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="10"/>
       <c r="C13" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="10"/>
       <c r="C14" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="10"/>
       <c r="C15" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="3" t="s">
@@ -904,225 +1039,225 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="2:6">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="10"/>
+      <c r="C16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="10"/>
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="10"/>
+      <c r="C18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="11"/>
-      <c r="C17" s="4" t="s">
+      <c r="D19" s="7"/>
+      <c r="E19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="11"/>
+      <c r="C20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="2:6">
-      <c r="B18" s="10" t="s">
+      <c r="D20" s="6"/>
+      <c r="E20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="B19" s="10"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="3" t="s">
+      <c r="E21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="10"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="2:6">
-      <c r="B20" s="10"/>
-      <c r="C20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="B21" s="10"/>
-      <c r="C21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="B22" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F22" s="2"/>
+      <c r="E22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23" s="10"/>
       <c r="C23" s="3" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="2:6">
-      <c r="B24" s="11"/>
-      <c r="C24" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24" s="4"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="2:6">
-      <c r="B25" s="10" t="s">
-        <v>47</v>
-      </c>
+      <c r="B25" s="10"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F25" s="3"/>
+      <c r="D25" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26" s="10"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="3"/>
+      <c r="D26" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" s="10"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="3"/>
+      <c r="D27" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="28" spans="2:6">
-      <c r="B28" s="10"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F28" s="3"/>
+      <c r="B28" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" s="10"/>
-      <c r="C29" s="5"/>
+      <c r="C29" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D29" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="F29" s="3"/>
     </row>
     <row r="30" spans="2:6">
-      <c r="B30" s="10"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F30" s="3"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" spans="2:6">
-      <c r="B31" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="B31" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F31" s="2"/>
+      <c r="E31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="3"/>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" s="10"/>
-      <c r="C32" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="C32" s="5"/>
       <c r="D32" s="3" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="2:6">
       <c r="B33" s="10"/>
-      <c r="C33" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C33" s="5"/>
       <c r="D33" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>4</v>
@@ -1131,10 +1266,10 @@
     </row>
     <row r="34" spans="2:6">
       <c r="B34" s="10"/>
-      <c r="C34" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="E34" s="3" t="s">
         <v>2</v>
       </c>
@@ -1142,74 +1277,74 @@
     </row>
     <row r="35" spans="2:6">
       <c r="B35" s="10"/>
-      <c r="C35" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E35" s="3" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="2:6">
-      <c r="B36" s="11"/>
-      <c r="C36" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F36" s="4"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" spans="2:6">
-      <c r="B37" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F37" s="3"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="38" spans="2:6">
       <c r="B38" s="10"/>
-      <c r="C38" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F38" s="3"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="39" spans="2:6">
-      <c r="B39" s="10"/>
-      <c r="C39" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F39" s="3"/>
+      <c r="B39" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" s="2"/>
     </row>
     <row r="40" spans="2:6">
       <c r="B40" s="10"/>
       <c r="C40" s="3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>4</v>
@@ -1219,72 +1354,72 @@
     <row r="41" spans="2:6">
       <c r="B41" s="10"/>
       <c r="C41" s="3" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="2:6">
       <c r="B42" s="10"/>
-      <c r="C42" s="13" t="s">
-        <v>14</v>
+      <c r="C42" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="D42" s="5"/>
-      <c r="E42" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F42" s="13" t="s">
-        <v>68</v>
-      </c>
+      <c r="E42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42" s="3"/>
     </row>
     <row r="43" spans="2:6">
       <c r="B43" s="10"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F43" s="14"/>
+      <c r="C43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F43" s="3"/>
     </row>
     <row r="44" spans="2:6">
-      <c r="B44" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D44" s="7"/>
-      <c r="E44" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F44" s="2"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" s="3"/>
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="11"/>
-      <c r="C45" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F45" s="4"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="46" spans="2:6">
       <c r="B46" s="10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D46" s="5"/>
+      <c r="D46" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="E46" s="3" t="s">
         <v>2</v>
       </c>
@@ -1293,22 +1428,28 @@
     <row r="47" spans="2:6">
       <c r="B47" s="10"/>
       <c r="C47" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D47" s="5"/>
-      <c r="E47" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F47" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="48" spans="2:6">
       <c r="B48" s="10"/>
       <c r="C48" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D48" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="E48" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F48" s="3"/>
     </row>
@@ -1317,7 +1458,9 @@
       <c r="C49" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D49" s="5"/>
+      <c r="D49" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="E49" s="3" t="s">
         <v>4</v>
       </c>
@@ -1326,9 +1469,11 @@
     <row r="50" spans="2:6">
       <c r="B50" s="10"/>
       <c r="C50" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D50" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="E50" s="3" t="s">
         <v>2</v>
       </c>
@@ -1336,69 +1481,71 @@
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="10"/>
-      <c r="C51" s="3" t="s">
-        <v>15</v>
+      <c r="C51" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="D51" s="5"/>
-      <c r="E51" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F51" s="3"/>
+      <c r="E51" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="52" spans="2:6">
-      <c r="B52" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D52" s="7"/>
-      <c r="E52" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F52" s="2"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F52" s="14"/>
     </row>
     <row r="53" spans="2:6">
-      <c r="B53" s="11"/>
-      <c r="C53" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D53" s="6"/>
-      <c r="E53" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F53" s="4"/>
+      <c r="B53" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D53" s="7"/>
+      <c r="E53" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F53" s="2"/>
     </row>
     <row r="54" spans="2:6">
-      <c r="B54" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="3" t="s">
+      <c r="B54" s="11"/>
+      <c r="C54" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="6"/>
+      <c r="E54" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" s="4"/>
+    </row>
+    <row r="55" spans="2:6">
+      <c r="B55" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E54" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="2:6">
-      <c r="B55" s="10"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="D55" s="5"/>
       <c r="E55" s="3" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="F55" s="3"/>
     </row>
     <row r="56" spans="2:6">
       <c r="B56" s="10"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="C56" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D56" s="5"/>
       <c r="E56" s="3" t="s">
         <v>4</v>
       </c>
@@ -1406,78 +1553,225 @@
     </row>
     <row r="57" spans="2:6">
       <c r="B57" s="10"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C57" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D57" s="5"/>
       <c r="E57" s="3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F57" s="3"/>
     </row>
     <row r="58" spans="2:6">
       <c r="B58" s="10"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="3" t="s">
+      <c r="C58" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="2:6">
+      <c r="B59" s="10"/>
+      <c r="C59" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D59" s="5"/>
+      <c r="E59" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="2:6">
+      <c r="B60" s="10"/>
+      <c r="C60" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E58" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="2:6">
-      <c r="B59" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C59" s="7"/>
-      <c r="D59" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="2:6">
-      <c r="B60" s="11"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F60" s="4"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F60" s="3"/>
     </row>
     <row r="61" spans="2:6">
-      <c r="B61" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F61" s="3"/>
+      <c r="B61" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D61" s="7"/>
+      <c r="E61" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F61" s="2"/>
     </row>
     <row r="62" spans="2:6">
       <c r="B62" s="11"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="4" t="s">
+      <c r="C62" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D62" s="6"/>
+      <c r="E62" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F62" s="4"/>
+    </row>
+    <row r="63" spans="2:6">
+      <c r="B63" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C63" s="5"/>
+      <c r="D63" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="2:6">
+      <c r="B64" s="10"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="2:6">
+      <c r="B65" s="10"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66" spans="2:6">
+      <c r="B66" s="10"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F66" s="3"/>
+    </row>
+    <row r="67" spans="2:6">
+      <c r="B67" s="10"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68" spans="2:6">
+      <c r="B68" s="10"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E68" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F68" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6">
+      <c r="B69" s="10"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E69" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="F69" s="17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6">
+      <c r="B70" s="10"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E70" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F70" s="17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6">
+      <c r="B71" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C71" s="7"/>
+      <c r="D71" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E71" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F71" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6">
+      <c r="B72" s="11"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E72" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F72" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6">
+      <c r="B73" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E73" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F73" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6">
+      <c r="B74" s="11"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E62" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F62" s="4"/>
+      <c r="E74" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F74" s="16" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:F62">
-    <filterColumn colId="2"/>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1487,7 +1781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>

</xml_diff>